<commit_message>
Improve chart axis labels for production data
Update y-axis titles in `app.py` and `templates/wykres.html` from empty strings to 'Produkcja dzienna' and 'Produkcja narastająca' respectively.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 5625db9c-3aa2-49fc-b31c-96cb5ad0b624
Replit-Commit-Checkpoint-Type: full_checkpoint
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/833c1fe7-c158-49af-9cc9-612b8ea8ed9d/5625db9c-3aa2-49fc-b31c-96cb5ad0b624/sR2TY3m
</commit_message>
<xml_diff>
--- a/Export.xlsx
+++ b/Export.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://storaenso-my.sharepoint.com/personal/dariusz_buchalski_storaenso_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1AA90C73-5763-4926-B440-3A8A8FDD37FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{1AA90C73-5763-4926-B440-3A8A8FDD37FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E3C4F48-10F5-406A-98A7-785C76959CF2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BF59FA5A-8DA5-47D9-B6C7-E39A087C6F68}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="729" uniqueCount="6">
   <si>
     <t>Dzienne</t>
   </si>
@@ -431,12 +431,12 @@
   <dimension ref="A1:AH67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -534,7 +534,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -622,8 +622,8 @@
       <c r="AC2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD2" s="1" t="s">
-        <v>2</v>
+      <c r="AD2" s="1">
+        <v>1918.826086956522</v>
       </c>
       <c r="AE2" s="1" t="s">
         <v>2</v>
@@ -638,7 +638,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -726,8 +726,8 @@
       <c r="AC3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD3" s="1" t="s">
-        <v>2</v>
+      <c r="AD3" s="1">
+        <v>993.26086956521749</v>
       </c>
       <c r="AE3" s="1" t="s">
         <v>2</v>
@@ -742,7 +742,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -830,8 +830,8 @@
       <c r="AC4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD4" s="1" t="s">
-        <v>2</v>
+      <c r="AD4" s="1">
+        <v>1727.0869565217392</v>
       </c>
       <c r="AE4" s="1" t="s">
         <v>2</v>
@@ -846,7 +846,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -935,22 +935,22 @@
         <v>2355.6185790768332</v>
       </c>
       <c r="AD5" s="1">
-        <v>2355.6185790768332</v>
+        <v>2328.3597883597881</v>
       </c>
       <c r="AE5" s="1">
-        <v>2355.6185790768332</v>
+        <v>2328.3597883597881</v>
       </c>
       <c r="AF5" s="1">
-        <v>2355.6185790768332</v>
+        <v>2328.3597883597881</v>
       </c>
       <c r="AG5" s="1">
-        <v>2355.6185790768332</v>
+        <v>2328.3597883597881</v>
       </c>
       <c r="AH5" s="1">
-        <v>2355.6185790768332</v>
+        <v>2328.3597883597881</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1039,22 +1039,22 @@
         <v>2398.4365558912382</v>
       </c>
       <c r="AD6" s="1">
-        <v>2398.4365558912382</v>
+        <v>2321.5230842455971</v>
       </c>
       <c r="AE6" s="1">
-        <v>2398.4365558912382</v>
+        <v>2321.5230842455971</v>
       </c>
       <c r="AF6" s="1">
-        <v>2398.4365558912382</v>
+        <v>2321.5230842455971</v>
       </c>
       <c r="AG6" s="1">
-        <v>2398.4365558912382</v>
+        <v>2321.5230842455971</v>
       </c>
       <c r="AH6" s="1">
-        <v>2398.4365558912382</v>
+        <v>2321.5230842455971</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1143,22 +1143,22 @@
         <v>2631.4420432220045</v>
       </c>
       <c r="AD7" s="1">
-        <v>2631.4420432220045</v>
+        <v>2556.4864864864867</v>
       </c>
       <c r="AE7" s="1">
-        <v>2631.4420432220045</v>
+        <v>2556.4864864864867</v>
       </c>
       <c r="AF7" s="1">
-        <v>2631.4420432220045</v>
+        <v>2556.4864864864867</v>
       </c>
       <c r="AG7" s="1">
-        <v>2631.4420432220045</v>
+        <v>2556.4864864864867</v>
       </c>
       <c r="AH7" s="1">
-        <v>2631.4420432220045</v>
+        <v>2556.4864864864867</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -1246,8 +1246,8 @@
       <c r="AC8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD8" s="1" t="s">
-        <v>2</v>
+      <c r="AD8" s="1">
+        <v>2439.2147806004618</v>
       </c>
       <c r="AE8" s="1" t="s">
         <v>2</v>
@@ -1262,7 +1262,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>0</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1487,94 +1487,94 @@
         <v>1959.1011235955054</v>
       </c>
       <c r="F11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="G11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="H11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="I11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="J11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="K11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="L11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="M11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="N11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="O11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="P11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="Q11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="R11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="S11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="T11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="U11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="V11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="W11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="X11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="Y11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="Z11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="AA11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="AB11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="AC11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="AD11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="AE11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="AF11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="AG11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
       <c r="AH11" s="1">
-        <v>1878.9528535980148</v>
+        <v>1933.3094331167379</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>1987.8755364806866</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>1496.5334063526836</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>0</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>561.25</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -2302,7 +2302,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>707.25</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -2494,8 +2494,8 @@
       <c r="AC20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD20" s="1" t="s">
-        <v>2</v>
+      <c r="AD20" s="1">
+        <v>2677.6956521739135</v>
       </c>
       <c r="AE20" s="1" t="s">
         <v>2</v>
@@ -2510,7 +2510,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>0</v>
       </c>
@@ -2598,8 +2598,8 @@
       <c r="AC21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD21" s="1" t="s">
-        <v>2</v>
+      <c r="AD21" s="1">
+        <v>2487.130434782609</v>
       </c>
       <c r="AE21" s="1" t="s">
         <v>2</v>
@@ -2614,7 +2614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
@@ -2702,8 +2702,8 @@
       <c r="AC22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD22" s="1" t="s">
-        <v>2</v>
+      <c r="AD22" s="1">
+        <v>2471.5813953488373</v>
       </c>
       <c r="AE22" s="1" t="s">
         <v>2</v>
@@ -2718,7 +2718,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
@@ -2807,22 +2807,22 @@
         <v>3558.6703953222327</v>
       </c>
       <c r="AD23" s="1">
-        <v>3558.6703953222327</v>
+        <v>3510.0036027380816</v>
       </c>
       <c r="AE23" s="1">
-        <v>3558.6703953222327</v>
+        <v>3510.0036027380816</v>
       </c>
       <c r="AF23" s="1">
-        <v>3558.6703953222327</v>
+        <v>3510.0036027380816</v>
       </c>
       <c r="AG23" s="1">
-        <v>3558.6703953222327</v>
+        <v>3510.0036027380816</v>
       </c>
       <c r="AH23" s="1">
-        <v>3558.6703953222327</v>
+        <v>3510.0036027380816</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
@@ -2911,22 +2911,22 @@
         <v>3051.2904372555981</v>
       </c>
       <c r="AD24" s="1">
-        <v>3051.2904372555981</v>
+        <v>3022.1283290257329</v>
       </c>
       <c r="AE24" s="1">
-        <v>3051.2904372555981</v>
+        <v>3022.1283290257329</v>
       </c>
       <c r="AF24" s="1">
-        <v>3051.2904372555981</v>
+        <v>3022.1283290257329</v>
       </c>
       <c r="AG24" s="1">
-        <v>3051.2904372555981</v>
+        <v>3022.1283290257329</v>
       </c>
       <c r="AH24" s="1">
-        <v>3051.2904372555981</v>
+        <v>3022.1283290257329</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
@@ -3015,22 +3015,22 @@
         <v>3409.6504339440698</v>
       </c>
       <c r="AD25" s="1">
-        <v>3409.6504339440698</v>
+        <v>3363.4242493696997</v>
       </c>
       <c r="AE25" s="1">
-        <v>3409.6504339440698</v>
+        <v>3363.4242493696997</v>
       </c>
       <c r="AF25" s="1">
-        <v>3409.6504339440698</v>
+        <v>3363.4242493696997</v>
       </c>
       <c r="AG25" s="1">
-        <v>3409.6504339440698</v>
+        <v>3363.4242493696997</v>
       </c>
       <c r="AH25" s="1">
-        <v>3409.6504339440698</v>
+        <v>3363.4242493696997</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -3118,8 +3118,8 @@
       <c r="AC26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD26" s="1" t="s">
-        <v>2</v>
+      <c r="AD26" s="1">
+        <v>2544.3913043478265</v>
       </c>
       <c r="AE26" s="1" t="s">
         <v>2</v>
@@ -3134,7 +3134,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>0</v>
       </c>
@@ -3222,8 +3222,8 @@
       <c r="AC27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD27" s="1" t="s">
-        <v>2</v>
+      <c r="AD27" s="1">
+        <v>1377.2207084468666</v>
       </c>
       <c r="AE27" s="1" t="s">
         <v>2</v>
@@ -3238,7 +3238,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>0</v>
       </c>
@@ -3326,8 +3326,8 @@
       <c r="AC28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD28" s="1" t="s">
-        <v>2</v>
+      <c r="AD28" s="1">
+        <v>2113.7647058823532</v>
       </c>
       <c r="AE28" s="1" t="s">
         <v>2</v>
@@ -3342,7 +3342,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
@@ -3431,22 +3431,22 @@
         <v>2140.5995873285592</v>
       </c>
       <c r="AD29" s="1">
-        <v>2140.5995873285592</v>
+        <v>2161.9519484998277</v>
       </c>
       <c r="AE29" s="1">
-        <v>2140.5995873285592</v>
+        <v>2161.9519484998277</v>
       </c>
       <c r="AF29" s="1">
-        <v>2140.5995873285592</v>
+        <v>2161.9519484998277</v>
       </c>
       <c r="AG29" s="1">
-        <v>2140.5995873285592</v>
+        <v>2161.9519484998277</v>
       </c>
       <c r="AH29" s="1">
-        <v>2140.5995873285592</v>
+        <v>2161.9519484998277</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
@@ -3535,22 +3535,22 @@
         <v>1815.3190029727873</v>
       </c>
       <c r="AD30" s="1">
-        <v>1815.3190029727873</v>
+        <v>1797.6758476901127</v>
       </c>
       <c r="AE30" s="1">
-        <v>1815.3190029727873</v>
+        <v>1797.6758476901127</v>
       </c>
       <c r="AF30" s="1">
-        <v>1815.3190029727873</v>
+        <v>1797.6758476901127</v>
       </c>
       <c r="AG30" s="1">
-        <v>1815.3190029727873</v>
+        <v>1797.6758476901127</v>
       </c>
       <c r="AH30" s="1">
-        <v>1815.3190029727873</v>
+        <v>1797.6758476901127</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
@@ -3639,22 +3639,22 @@
         <v>2632.5425330812855</v>
       </c>
       <c r="AD31" s="1">
-        <v>2632.5425330812855</v>
+        <v>2612.507950931395</v>
       </c>
       <c r="AE31" s="1">
-        <v>2632.5425330812855</v>
+        <v>2612.507950931395</v>
       </c>
       <c r="AF31" s="1">
-        <v>2632.5425330812855</v>
+        <v>2612.507950931395</v>
       </c>
       <c r="AG31" s="1">
-        <v>2632.5425330812855</v>
+        <v>2612.507950931395</v>
       </c>
       <c r="AH31" s="1">
-        <v>2632.5425330812855</v>
+        <v>2612.507950931395</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>0</v>
       </c>
@@ -3742,8 +3742,8 @@
       <c r="AC32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD32" s="1" t="s">
-        <v>2</v>
+      <c r="AD32" s="1">
+        <v>1358.3259911894274</v>
       </c>
       <c r="AE32" s="1" t="s">
         <v>2</v>
@@ -3758,7 +3758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>0</v>
       </c>
@@ -3846,8 +3846,8 @@
       <c r="AC33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD33" s="1" t="s">
-        <v>2</v>
+      <c r="AD33" s="1">
+        <v>1290.7826086956522</v>
       </c>
       <c r="AE33" s="1" t="s">
         <v>2</v>
@@ -3862,7 +3862,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -3950,8 +3950,8 @@
       <c r="AC34" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD34" s="1" t="s">
-        <v>2</v>
+      <c r="AD34" s="1">
+        <v>1770.7826086956522</v>
       </c>
       <c r="AE34" s="1" t="s">
         <v>2</v>
@@ -3966,7 +3966,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>5</v>
       </c>
@@ -4055,22 +4055,22 @@
         <v>1294.7439298102429</v>
       </c>
       <c r="AD35" s="1">
-        <v>1294.7439298102429</v>
+        <v>1300.1344537815128</v>
       </c>
       <c r="AE35" s="1">
-        <v>1294.7439298102429</v>
+        <v>1300.1344537815128</v>
       </c>
       <c r="AF35" s="1">
-        <v>1294.7439298102429</v>
+        <v>1300.1344537815128</v>
       </c>
       <c r="AG35" s="1">
-        <v>1294.7439298102429</v>
+        <v>1300.1344537815128</v>
       </c>
       <c r="AH35" s="1">
-        <v>1294.7439298102429</v>
+        <v>1300.1344537815128</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
@@ -4159,22 +4159,22 @@
         <v>1305.5505819158461</v>
       </c>
       <c r="AD36" s="1">
-        <v>1305.5505819158461</v>
+        <v>1304.172077922078</v>
       </c>
       <c r="AE36" s="1">
-        <v>1305.5505819158461</v>
+        <v>1304.172077922078</v>
       </c>
       <c r="AF36" s="1">
-        <v>1305.5505819158461</v>
+        <v>1304.172077922078</v>
       </c>
       <c r="AG36" s="1">
-        <v>1305.5505819158461</v>
+        <v>1304.172077922078</v>
       </c>
       <c r="AH36" s="1">
-        <v>1305.5505819158461</v>
+        <v>1304.172077922078</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
@@ -4263,22 +4263,22 @@
         <v>1148.5960334029226</v>
       </c>
       <c r="AD37" s="1">
-        <v>1148.5960334029226</v>
+        <v>1215.279589934762</v>
       </c>
       <c r="AE37" s="1">
-        <v>1148.5960334029226</v>
+        <v>1215.279589934762</v>
       </c>
       <c r="AF37" s="1">
-        <v>1148.5960334029226</v>
+        <v>1215.279589934762</v>
       </c>
       <c r="AG37" s="1">
-        <v>1148.5960334029226</v>
+        <v>1215.279589934762</v>
       </c>
       <c r="AH37" s="1">
-        <v>1148.5960334029226</v>
+        <v>1215.279589934762</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>0</v>
       </c>
@@ -4366,8 +4366,8 @@
       <c r="AC38" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD38" s="1" t="s">
-        <v>2</v>
+      <c r="AD38" s="1">
+        <v>570.41474654377885</v>
       </c>
       <c r="AE38" s="1" t="s">
         <v>2</v>
@@ -4382,7 +4382,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>0</v>
       </c>
@@ -4470,8 +4470,8 @@
       <c r="AC39" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD39" s="1" t="s">
-        <v>2</v>
+      <c r="AD39" s="1">
+        <v>1249.0434782608697</v>
       </c>
       <c r="AE39" s="1" t="s">
         <v>2</v>
@@ -4486,7 +4486,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>0</v>
       </c>
@@ -4590,7 +4590,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>5</v>
       </c>
@@ -4679,22 +4679,22 @@
         <v>1861.6869728209936</v>
       </c>
       <c r="AD41" s="1">
-        <v>1861.6869728209936</v>
+        <v>1643.4579439252338</v>
       </c>
       <c r="AE41" s="1">
-        <v>1861.6869728209936</v>
+        <v>1643.4579439252338</v>
       </c>
       <c r="AF41" s="1">
-        <v>1861.6869728209936</v>
+        <v>1643.4579439252338</v>
       </c>
       <c r="AG41" s="1">
-        <v>1861.6869728209936</v>
+        <v>1643.4579439252338</v>
       </c>
       <c r="AH41" s="1">
-        <v>1861.6869728209936</v>
+        <v>1643.4579439252338</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>5</v>
       </c>
@@ -4783,22 +4783,22 @@
         <v>1871.6698841698842</v>
       </c>
       <c r="AD42" s="1">
-        <v>1871.6698841698842</v>
+        <v>1758.5545023696682</v>
       </c>
       <c r="AE42" s="1">
-        <v>1871.6698841698842</v>
+        <v>1758.5545023696682</v>
       </c>
       <c r="AF42" s="1">
-        <v>1871.6698841698842</v>
+        <v>1758.5545023696682</v>
       </c>
       <c r="AG42" s="1">
-        <v>1871.6698841698842</v>
+        <v>1758.5545023696682</v>
       </c>
       <c r="AH42" s="1">
-        <v>1871.6698841698842</v>
+        <v>1758.5545023696682</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>5</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>1552.0062695924767</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>0</v>
       </c>
@@ -4990,8 +4990,8 @@
       <c r="AC44" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD44" s="1" t="s">
-        <v>2</v>
+      <c r="AD44" s="1">
+        <v>6876.3380281690133</v>
       </c>
       <c r="AE44" s="1" t="s">
         <v>2</v>
@@ -5006,7 +5006,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>0</v>
       </c>
@@ -5094,8 +5094,8 @@
       <c r="AC45" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD45" s="1" t="s">
-        <v>2</v>
+      <c r="AD45" s="1">
+        <v>4978.7264150943402</v>
       </c>
       <c r="AE45" s="1" t="s">
         <v>2</v>
@@ -5110,7 +5110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>0</v>
       </c>
@@ -5198,8 +5198,8 @@
       <c r="AC46" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD46" s="1" t="s">
-        <v>2</v>
+      <c r="AD46" s="1">
+        <v>3610.864864864865</v>
       </c>
       <c r="AE46" s="1" t="s">
         <v>2</v>
@@ -5214,7 +5214,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>5</v>
       </c>
@@ -5303,22 +5303,22 @@
         <v>3807.8588807785882</v>
       </c>
       <c r="AD47" s="1">
-        <v>3807.8588807785882</v>
+        <v>3948.3606345930598</v>
       </c>
       <c r="AE47" s="1">
-        <v>3807.8588807785882</v>
+        <v>3948.3606345930598</v>
       </c>
       <c r="AF47" s="1">
-        <v>3807.8588807785882</v>
+        <v>3948.3606345930598</v>
       </c>
       <c r="AG47" s="1">
-        <v>3807.8588807785882</v>
+        <v>3948.3606345930598</v>
       </c>
       <c r="AH47" s="1">
-        <v>3807.8588807785882</v>
+        <v>3948.3606345930598</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>5</v>
       </c>
@@ -5407,22 +5407,22 @@
         <v>3559.3594306049818</v>
       </c>
       <c r="AD48" s="1">
-        <v>3559.3594306049818</v>
+        <v>3634.4825864436398</v>
       </c>
       <c r="AE48" s="1">
-        <v>3559.3594306049818</v>
+        <v>3634.4825864436398</v>
       </c>
       <c r="AF48" s="1">
-        <v>3559.3594306049818</v>
+        <v>3634.4825864436398</v>
       </c>
       <c r="AG48" s="1">
-        <v>3559.3594306049818</v>
+        <v>3634.4825864436398</v>
       </c>
       <c r="AH48" s="1">
-        <v>3559.3594306049818</v>
+        <v>3634.4825864436398</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>5</v>
       </c>
@@ -5511,22 +5511,22 @@
         <v>4056.5583673469382</v>
       </c>
       <c r="AD49" s="1">
-        <v>4056.5583673469382</v>
+        <v>4031.1685912240187</v>
       </c>
       <c r="AE49" s="1">
-        <v>4056.5583673469382</v>
+        <v>4031.1685912240187</v>
       </c>
       <c r="AF49" s="1">
-        <v>4056.5583673469382</v>
+        <v>4031.1685912240187</v>
       </c>
       <c r="AG49" s="1">
-        <v>4056.5583673469382</v>
+        <v>4031.1685912240187</v>
       </c>
       <c r="AH49" s="1">
-        <v>4056.5583673469382</v>
+        <v>4031.1685912240187</v>
       </c>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>0</v>
       </c>
@@ -5614,8 +5614,8 @@
       <c r="AC50" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD50" s="1" t="s">
-        <v>2</v>
+      <c r="AD50" s="1">
+        <v>644.73913043478262</v>
       </c>
       <c r="AE50" s="1" t="s">
         <v>2</v>
@@ -5630,7 +5630,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>0</v>
       </c>
@@ -5718,8 +5718,8 @@
       <c r="AC51" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD51" s="1" t="s">
-        <v>2</v>
+      <c r="AD51" s="1">
+        <v>758.75000000000011</v>
       </c>
       <c r="AE51" s="1" t="s">
         <v>2</v>
@@ -5734,7 +5734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>0</v>
       </c>
@@ -5838,7 +5838,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>5</v>
       </c>
@@ -5927,22 +5927,22 @@
         <v>5408.7750791974668</v>
       </c>
       <c r="AD53" s="1">
-        <v>5408.7750791974668</v>
+        <v>5051.9765548681216</v>
       </c>
       <c r="AE53" s="1">
-        <v>5408.7750791974668</v>
+        <v>5051.9765548681216</v>
       </c>
       <c r="AF53" s="1">
-        <v>5408.7750791974668</v>
+        <v>5051.9765548681216</v>
       </c>
       <c r="AG53" s="1">
-        <v>5408.7750791974668</v>
+        <v>5051.9765548681216</v>
       </c>
       <c r="AH53" s="1">
-        <v>5408.7750791974668</v>
+        <v>5051.9765548681216</v>
       </c>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>5</v>
       </c>
@@ -6031,22 +6031,22 @@
         <v>4916.2946708463951</v>
       </c>
       <c r="AD54" s="1">
-        <v>4916.2946708463951</v>
+        <v>4652.6335877862593</v>
       </c>
       <c r="AE54" s="1">
-        <v>4916.2946708463951</v>
+        <v>4652.6335877862593</v>
       </c>
       <c r="AF54" s="1">
-        <v>4916.2946708463951</v>
+        <v>4652.6335877862593</v>
       </c>
       <c r="AG54" s="1">
-        <v>4916.2946708463951</v>
+        <v>4652.6335877862593</v>
       </c>
       <c r="AH54" s="1">
-        <v>4916.2946708463951</v>
+        <v>4652.6335877862593</v>
       </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>5</v>
       </c>
@@ -6150,7 +6150,7 @@
         <v>7571.6310016184134</v>
       </c>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>0</v>
       </c>
@@ -6254,7 +6254,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>0</v>
       </c>
@@ -6342,8 +6342,8 @@
       <c r="AC57" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD57" s="1" t="s">
-        <v>2</v>
+      <c r="AD57" s="1">
+        <v>2290.3174603174602</v>
       </c>
       <c r="AE57" s="1" t="s">
         <v>2</v>
@@ -6358,7 +6358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
@@ -6446,8 +6446,8 @@
       <c r="AC58" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD58" s="1" t="s">
-        <v>2</v>
+      <c r="AD58" s="1">
+        <v>3766.5198237885465</v>
       </c>
       <c r="AE58" s="1" t="s">
         <v>2</v>
@@ -6462,7 +6462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>5</v>
       </c>
@@ -6566,7 +6566,7 @@
         <v>2166.6626268747159</v>
       </c>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>5</v>
       </c>
@@ -6655,22 +6655,22 @@
         <v>2331.9311030142435</v>
       </c>
       <c r="AD60" s="1">
-        <v>2331.9311030142435</v>
+        <v>2329.4794264339157</v>
       </c>
       <c r="AE60" s="1">
-        <v>2331.9311030142435</v>
+        <v>2329.4794264339157</v>
       </c>
       <c r="AF60" s="1">
-        <v>2331.9311030142435</v>
+        <v>2329.4794264339157</v>
       </c>
       <c r="AG60" s="1">
-        <v>2331.9311030142435</v>
+        <v>2329.4794264339157</v>
       </c>
       <c r="AH60" s="1">
-        <v>2331.9311030142435</v>
+        <v>2329.4794264339157</v>
       </c>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>5</v>
       </c>
@@ -6759,22 +6759,22 @@
         <v>2598.3872590108963</v>
       </c>
       <c r="AD61" s="1">
-        <v>2598.3872590108963</v>
+        <v>2681.0063872877395</v>
       </c>
       <c r="AE61" s="1">
-        <v>2598.3872590108963</v>
+        <v>2681.0063872877395</v>
       </c>
       <c r="AF61" s="1">
-        <v>2598.3872590108963</v>
+        <v>2681.0063872877395</v>
       </c>
       <c r="AG61" s="1">
-        <v>2598.3872590108963</v>
+        <v>2681.0063872877395</v>
       </c>
       <c r="AH61" s="1">
-        <v>2598.3872590108963</v>
+        <v>2681.0063872877395</v>
       </c>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>0</v>
       </c>
@@ -6862,8 +6862,8 @@
       <c r="AC62" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD62" s="1" t="s">
-        <v>2</v>
+      <c r="AD62" s="1">
+        <v>2262.5720620842571</v>
       </c>
       <c r="AE62" s="1" t="s">
         <v>2</v>
@@ -6878,7 +6878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>0</v>
       </c>
@@ -6966,8 +6966,8 @@
       <c r="AC63" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD63" s="1" t="s">
-        <v>2</v>
+      <c r="AD63" s="1">
+        <v>4338.913043478261</v>
       </c>
       <c r="AE63" s="1" t="s">
         <v>2</v>
@@ -6982,7 +6982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
@@ -7070,8 +7070,8 @@
       <c r="AC64" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="AD64" s="1" t="s">
-        <v>2</v>
+      <c r="AD64" s="1">
+        <v>2483.4782608695655</v>
       </c>
       <c r="AE64" s="1" t="s">
         <v>2</v>
@@ -7086,7 +7086,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>5</v>
       </c>
@@ -7175,22 +7175,22 @@
         <v>2980.6941250261343</v>
       </c>
       <c r="AD65" s="1">
-        <v>2980.6941250261343</v>
+        <v>2918.8154375238823</v>
       </c>
       <c r="AE65" s="1">
-        <v>2980.6941250261343</v>
+        <v>2918.8154375238823</v>
       </c>
       <c r="AF65" s="1">
-        <v>2980.6941250261343</v>
+        <v>2918.8154375238823</v>
       </c>
       <c r="AG65" s="1">
-        <v>2980.6941250261343</v>
+        <v>2918.8154375238823</v>
       </c>
       <c r="AH65" s="1">
-        <v>2980.6941250261343</v>
+        <v>2918.8154375238823</v>
       </c>
     </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>5</v>
       </c>
@@ -7279,22 +7279,22 @@
         <v>2272.0473696196773</v>
       </c>
       <c r="AD66" s="1">
-        <v>2272.0473696196773</v>
+        <v>2468.0395794681513</v>
       </c>
       <c r="AE66" s="1">
-        <v>2272.0473696196773</v>
+        <v>2468.0395794681513</v>
       </c>
       <c r="AF66" s="1">
-        <v>2272.0473696196773</v>
+        <v>2468.0395794681513</v>
       </c>
       <c r="AG66" s="1">
-        <v>2272.0473696196773</v>
+        <v>2468.0395794681513</v>
       </c>
       <c r="AH66" s="1">
-        <v>2272.0473696196773</v>
+        <v>2468.0395794681513</v>
       </c>
     </row>
-    <row r="67" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>5</v>
       </c>
@@ -7383,19 +7383,19 @@
         <v>2773.5306122448983</v>
       </c>
       <c r="AD67" s="1">
-        <v>2773.5306122448983</v>
+        <v>2748.6380597014922</v>
       </c>
       <c r="AE67" s="1">
-        <v>2773.5306122448983</v>
+        <v>2748.6380597014922</v>
       </c>
       <c r="AF67" s="1">
-        <v>2773.5306122448983</v>
+        <v>2748.6380597014922</v>
       </c>
       <c r="AG67" s="1">
-        <v>2773.5306122448983</v>
+        <v>2748.6380597014922</v>
       </c>
       <c r="AH67" s="1">
-        <v>2773.5306122448983</v>
+        <v>2748.6380597014922</v>
       </c>
     </row>
   </sheetData>

</xml_diff>